<commit_message>
update labels and contaminant literature
</commit_message>
<xml_diff>
--- a/bin/contaminant_literature.xlsx
+++ b/bin/contaminant_literature.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angelasun/Downloads/contamination-data/bin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21D9E25-DA61-8F4D-A834-21DFEBB1BD52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DB0A96-509E-6A4C-818B-25F50BB57151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23700" yWindow="5180" windowWidth="27640" windowHeight="16940" xr2:uid="{4822B3BB-0C93-524F-83D5-E831C419493D}"/>
+    <workbookView xWindow="10320" yWindow="4560" windowWidth="27640" windowHeight="16940" xr2:uid="{4822B3BB-0C93-524F-83D5-E831C419493D}"/>
   </bookViews>
   <sheets>
     <sheet name="genus_table" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="547">
   <si>
     <t>Pathogenicity</t>
   </si>
@@ -1387,9 +1387,6 @@
     <t>gut,resp_tract,mouth</t>
   </si>
   <si>
-    <t>4,15</t>
-  </si>
-  <si>
     <t>gut,resp_tract</t>
   </si>
   <si>
@@ -1534,9 +1531,6 @@
     <t>13,15</t>
   </si>
   <si>
-    <t>13,37</t>
-  </si>
-  <si>
     <t>15,39</t>
   </si>
   <si>
@@ -1567,9 +1561,6 @@
     <t>mouth,soft_tissue</t>
   </si>
   <si>
-    <t>34, 38</t>
-  </si>
-  <si>
     <t>pollen</t>
   </si>
   <si>
@@ -1592,6 +1583,102 @@
   </si>
   <si>
     <t>Luo, J., Zhao, T., Su, W., Liu, F., Xu, Y. and Li, Z., 2025. Relationship of Mogibacterium in the gut microbiota with early-stage lung cancer. Journal of Applied Microbiology, 136(6), p.lxaf130.</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Könönen, E., Fteita, D., Gursoy, U.K. and Gursoy, M., 2022. Prevotella species as oral residents and infectious agents with potential impact on systemic conditions. Journal of Oral Microbiology, 14(1), p.2079814.</t>
+  </si>
+  <si>
+    <t>4,15,73</t>
+  </si>
+  <si>
+    <t>13,37,74</t>
+  </si>
+  <si>
+    <t>Yuan, C., Yin, Z., Wang, J., Qian, C., Wei, Y., Zhang, S., Jiang, L. and Liu, B., 2019. Comparative genomic analysis of Citrobacter and key genes essential for the pathogenicity of Citrobacter koseri. Frontiers in Microbiology, 10, p.2774.</t>
+  </si>
+  <si>
+    <t>Photobacterium</t>
+  </si>
+  <si>
+    <t>Labella, A.M., Arahal, D.R., Castro, D., Lemos, M.L. and Borrego, J.J., 2017. Revisiting the genus Photobacterium: taxonomy, ecology and pathogenesis. Int Microbiol, 20(1), pp.1-10.</t>
+  </si>
+  <si>
+    <t>Pectobacteria</t>
+  </si>
+  <si>
+    <t>Davidsson, P.R., Kariola, T., Niemi, O. and Palva, E.T., 2013. Pathogenicity of and plant immunity to soft rot pectobacteria. Frontiers in plant science, 4, p.191.</t>
+  </si>
+  <si>
+    <t>Deschaght P, Janssens M, Vaneechoutte M, Wauters G. 2012. Psychrobacter isolates of human origin, other than Psychrobacter phenylpyruvicus, are predominantly Psychrobacter faecalis and Psychrobacter pulmonis, with emended description of P faecalis. Int J Syst Evol Microbiol 62:671–674.</t>
+  </si>
+  <si>
+    <t>34,38</t>
+  </si>
+  <si>
+    <t>Welter, D.K., Ruaud, A., Henseler, Z.M., De Jong, H.N., Van Coeverden de Groot, P., Michaux, J., Gormezano, L., Waters, J.L., Youngblut, N.D. and Ley, R.E., 2021. Free-living, psychrotrophic bacteria of the genus psychrobacter are descendants of pathobionts. Msystems, 6(2), pp.10-1128.</t>
+  </si>
+  <si>
+    <t>4,77,78</t>
+  </si>
+  <si>
+    <t>Makizumi, Y., Igarashi, M., Gotoh, K., Murao, K., Yamamoto, M., Udonsri, N., Ochiai, H., Thummabenjapone, P. and Kaku, H., 2011. Genetic diversity and pathogenicity of cucurbit-associated Acidovorax. Journal of General Plant Pathology, 77(1), pp.24-32.</t>
+  </si>
+  <si>
+    <t>4,79</t>
+  </si>
+  <si>
+    <t>Letek, M., Gonzalez, P., MacArthur, I., Rodríguez, H., Freeman, T.C., Valero-Rello, A., Blanco, M., Buckley, T., Cherevach, I., Fahey, R. and Hapeshi, A., 2010. The genome of a pathogenic Rhodococcus: cooptive virulence underpinned by key gene acquisitions. PLoS genetics, 6(9), p.e1001145.</t>
+  </si>
+  <si>
+    <t>4,80</t>
+  </si>
+  <si>
+    <t>sterile_water,extraction_kit</t>
+  </si>
+  <si>
+    <t>4,81</t>
+  </si>
+  <si>
+    <t>Ghafari, S., Alavi, S.M. and Khaghani, S., 2024. Potentially pathogenic culturable bacteria in hemodialysis waters. BMC microbiology, 24(1), p.276.</t>
+  </si>
+  <si>
+    <t>Caproicibacterium</t>
+  </si>
+  <si>
+    <t>Zeng, C., Zeng, X., Xia, S. and Ye, G., 2024. Caproicibacterium argilliputei sp. nov., a novel caproic acid producing anaerobic bacterium isolated from pit clay. International Journal of Systematic and Evolutionary Microbiology, 74(1), p.006246.</t>
+  </si>
+  <si>
+    <t>Algoriphagus</t>
+  </si>
+  <si>
+    <t>Ali, S., Xie, J., Zada, S., Hu, Z., Zhang, Y., Cai, R. and Wang, H., 2022. Bacterial community structure and bacterial isolates having antimicrobial potential in shrimp pond aquaculture. AMB Express, 12(1), p.82.</t>
+  </si>
+  <si>
+    <t>Diaphorobacter</t>
+  </si>
+  <si>
+    <t>lung,gut</t>
+  </si>
+  <si>
+    <t>Ni, Y., Li, R., Shen, X., Yi, D., Ren, Y., Wang, F., Geng, Y. and You, Q., 2024. Diaphorobacter nitroreducens synergize with oxaliplatin to reduce tumor burden in mice with lung adenocarcinoma. Msystems, 9(4), pp.e01323-23.</t>
+  </si>
+  <si>
+    <t>Leclercia</t>
+  </si>
+  <si>
+    <t>food,gut,resp_tract,mucosa</t>
+  </si>
+  <si>
+    <t>Zayet, S., Lang, S., Garnier, P., Pierron, A., Plantin, J., Toko, L., Royer, P.Y., Villemain, M., Klopfenstein, T. and Gendrin, V., 2021. Leclercia adecarboxylata as emerging pathogen in human infections: clinical features and antimicrobial susceptibility testing. Pathogens, 10(11), p.1399.</t>
+  </si>
+  <si>
+    <t>Farhat, M., Alkharsah, K.R., Alkhamis, F.I. and Bukharie, H.A., 2019. Metagenomic study on the composition of culturable and non-culturable bacteria in tap water and biofilms at intensive care units. Journal of Water and Health, 17(1), pp.72-83.</t>
+  </si>
+  <si>
+    <t>4,86</t>
   </si>
 </sst>
 </file>
@@ -2004,10 +2091,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0E6A2D-7F01-AB49-9D89-C2DFE9B51DDB}">
-  <dimension ref="A1:F315"/>
+  <dimension ref="A1:F322"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A299" workbookViewId="0">
-      <selection activeCell="B333" sqref="B333"/>
+    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
+      <selection activeCell="I314" sqref="I314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2040,7 +2127,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>16</v>
@@ -2615,14 +2702,17 @@
       <c r="A38" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="3">
-        <v>4</v>
+      <c r="F38" s="3" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -2743,6 +2833,9 @@
       <c r="A48" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
       <c r="D48" t="s">
         <v>448</v>
       </c>
@@ -2750,7 +2843,7 @@
         <v>8</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>449</v>
+        <v>517</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2772,13 +2865,13 @@
         <v>6</v>
       </c>
       <c r="D50" t="s">
+        <v>449</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="3" t="s">
         <v>450</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
@@ -2817,7 +2910,7 @@
         <v>8</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
@@ -2837,7 +2930,7 @@
         <v>8</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2898,7 +2991,7 @@
         <v>8</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
@@ -2918,7 +3011,7 @@
         <v>8</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
@@ -2962,13 +3055,13 @@
         <v>6</v>
       </c>
       <c r="D64" t="s">
+        <v>455</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F64" s="3" t="s">
         <v>456</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
@@ -3015,13 +3108,13 @@
         <v>6</v>
       </c>
       <c r="D68" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
@@ -3082,7 +3175,7 @@
         <v>8</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -3121,7 +3214,7 @@
         <v>8</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
@@ -3132,13 +3225,13 @@
         <v>13</v>
       </c>
       <c r="D77" t="s">
+        <v>460</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F77" s="3" t="s">
         <v>461</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
@@ -3152,13 +3245,13 @@
         <v>29</v>
       </c>
       <c r="D78" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
@@ -3180,13 +3273,13 @@
         <v>6</v>
       </c>
       <c r="D80" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" s="3" t="s">
         <v>464</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
@@ -3352,7 +3445,7 @@
         <v>107</v>
       </c>
       <c r="D94" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>8</v>
@@ -3386,7 +3479,7 @@
         <v>8</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
@@ -3419,13 +3512,13 @@
         <v>43</v>
       </c>
       <c r="D99" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F99" s="3" t="s">
         <v>467</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
@@ -3621,7 +3714,7 @@
         <v>8</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
@@ -3660,7 +3753,7 @@
         <v>8</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
@@ -3677,7 +3770,7 @@
         <v>8</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
@@ -3688,7 +3781,7 @@
         <v>8</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
@@ -3710,18 +3803,21 @@
         <v>8</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>139</v>
       </c>
+      <c r="B124" t="s">
+        <v>3</v>
+      </c>
       <c r="E124" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F124" s="3">
-        <v>4</v>
+        <v>532</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
@@ -3813,7 +3909,7 @@
         <v>8</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
@@ -3827,7 +3923,7 @@
         <v>19</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
@@ -3888,7 +3984,7 @@
         <v>8</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
@@ -3905,7 +4001,7 @@
         <v>8</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
@@ -3919,7 +4015,7 @@
         <v>8</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
@@ -3933,7 +4029,7 @@
         <v>8</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
@@ -3945,7 +4041,7 @@
       </c>
       <c r="E141" s="3"/>
       <c r="F141" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
@@ -3966,11 +4062,17 @@
       <c r="A143" s="3" t="s">
         <v>159</v>
       </c>
+      <c r="B143" t="s">
+        <v>16</v>
+      </c>
+      <c r="C143" t="s">
+        <v>4</v>
+      </c>
       <c r="E143" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F143" s="3">
-        <v>4</v>
+      <c r="F143" s="3" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
@@ -3988,11 +4090,17 @@
       <c r="A145" s="3" t="s">
         <v>161</v>
       </c>
+      <c r="B145" t="s">
+        <v>515</v>
+      </c>
+      <c r="D145" t="s">
+        <v>267</v>
+      </c>
       <c r="E145" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F145" s="3">
-        <v>4</v>
+      <c r="F145" s="3" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
@@ -4020,7 +4128,7 @@
         <v>164</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
@@ -4048,7 +4156,7 @@
         <v>8</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
@@ -4059,7 +4167,7 @@
         <v>19</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
@@ -4114,7 +4222,7 @@
         <v>8</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
@@ -4166,7 +4274,7 @@
         <v>8</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
@@ -4199,7 +4307,7 @@
         <v>8</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
@@ -4238,13 +4346,13 @@
         <v>197</v>
       </c>
       <c r="D165" t="s">
+        <v>455</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F165" s="3" t="s">
         <v>456</v>
-      </c>
-      <c r="E165" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F165" s="3" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
@@ -4302,7 +4410,7 @@
         <v>8</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
@@ -4313,10 +4421,10 @@
         <v>43</v>
       </c>
       <c r="E171" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="F171" s="3" t="s">
         <v>483</v>
-      </c>
-      <c r="F171" s="3" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
@@ -4333,7 +4441,7 @@
         <v>19</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
@@ -4350,7 +4458,7 @@
         <v>19</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
@@ -4367,7 +4475,7 @@
         <v>8</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
@@ -4382,7 +4490,7 @@
       </c>
       <c r="E175" s="3"/>
       <c r="F175" s="3" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
@@ -4396,7 +4504,7 @@
         <v>8</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.2">
@@ -4421,11 +4529,11 @@
         <v>6</v>
       </c>
       <c r="D178" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E178" s="3"/>
       <c r="F178" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.2">
@@ -4442,18 +4550,27 @@
         <v>8</v>
       </c>
       <c r="F179" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
         <v>199</v>
       </c>
+      <c r="B180" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>267</v>
+      </c>
       <c r="E180" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F180" s="3">
-        <v>4</v>
+      <c r="F180" s="3" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.2">
@@ -4497,6 +4614,9 @@
       <c r="A184" s="3" t="s">
         <v>144</v>
       </c>
+      <c r="B184" t="s">
+        <v>515</v>
+      </c>
       <c r="C184" s="3" t="s">
         <v>4</v>
       </c>
@@ -4523,7 +4643,7 @@
         <v>164</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.2">
@@ -4655,7 +4775,7 @@
         <v>8</v>
       </c>
       <c r="F195" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.2">
@@ -4669,7 +4789,7 @@
         <v>197</v>
       </c>
       <c r="F196" s="3" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.2">
@@ -4697,7 +4817,7 @@
         <v>8</v>
       </c>
       <c r="F198" s="3" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.2">
@@ -4714,7 +4834,7 @@
         <v>19</v>
       </c>
       <c r="F199" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.2">
@@ -4745,7 +4865,7 @@
         <v>8</v>
       </c>
       <c r="F201" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.2">
@@ -4804,7 +4924,7 @@
         <v>8</v>
       </c>
       <c r="F205" s="3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.2">
@@ -4829,16 +4949,19 @@
         <v>197</v>
       </c>
       <c r="D207" t="s">
+        <v>493</v>
+      </c>
+      <c r="F207" s="3" t="s">
         <v>494</v>
-      </c>
-      <c r="F207" s="3" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
         <v>226</v>
       </c>
+      <c r="B208" t="s">
+        <v>515</v>
+      </c>
       <c r="E208" t="s">
         <v>21</v>
       </c>
@@ -4932,7 +5055,7 @@
         <v>19</v>
       </c>
       <c r="F215" s="3" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
@@ -4965,13 +5088,16 @@
         <v>110</v>
       </c>
       <c r="F218" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
         <v>237</v>
       </c>
+      <c r="B219" t="s">
+        <v>3</v>
+      </c>
       <c r="C219" t="s">
         <v>4</v>
       </c>
@@ -4982,7 +5108,7 @@
         <v>164</v>
       </c>
       <c r="F219" s="3" t="s">
-        <v>498</v>
+        <v>518</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
@@ -5004,7 +5130,7 @@
         <v>239</v>
       </c>
       <c r="C221" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="F221" s="3">
         <v>14</v>
@@ -5127,7 +5253,7 @@
         <v>110</v>
       </c>
       <c r="F230" s="3" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
@@ -5138,7 +5264,7 @@
         <v>54</v>
       </c>
       <c r="F231" s="3" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
@@ -5149,10 +5275,10 @@
         <v>6</v>
       </c>
       <c r="D232" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F232" s="3" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
@@ -5196,10 +5322,10 @@
         <v>13</v>
       </c>
       <c r="D236" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F236" s="3" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
@@ -5210,10 +5336,10 @@
         <v>6</v>
       </c>
       <c r="D237" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F237" s="3" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
@@ -5299,7 +5425,7 @@
         <v>6</v>
       </c>
       <c r="C244" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D244" t="s">
         <v>267</v>
@@ -5316,7 +5442,7 @@
         <v>6</v>
       </c>
       <c r="C245" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F245" s="3">
         <v>34</v>
@@ -5826,7 +5952,7 @@
         <v>4</v>
       </c>
       <c r="D281" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F281" s="3">
         <v>38</v>
@@ -5871,7 +5997,7 @@
         <v>110</v>
       </c>
       <c r="F284" s="3" t="s">
-        <v>509</v>
+        <v>525</v>
       </c>
     </row>
     <row r="285" spans="1:6" x14ac:dyDescent="0.2">
@@ -6008,7 +6134,7 @@
         <v>6</v>
       </c>
       <c r="C294" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D294" t="s">
         <v>135</v>
@@ -6146,7 +6272,7 @@
         <v>4</v>
       </c>
       <c r="D303" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F303" s="3">
         <v>59</v>
@@ -6160,7 +6286,7 @@
         <v>6</v>
       </c>
       <c r="C304" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F304" s="3">
         <v>65</v>
@@ -6174,7 +6300,7 @@
         <v>43</v>
       </c>
       <c r="D305" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F305" s="3">
         <v>66</v>
@@ -6188,7 +6314,7 @@
         <v>43</v>
       </c>
       <c r="D306" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F306" s="3">
         <v>66</v>
@@ -6202,7 +6328,7 @@
         <v>43</v>
       </c>
       <c r="D307" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F307" s="3">
         <v>66</v>
@@ -6216,7 +6342,7 @@
         <v>43</v>
       </c>
       <c r="D308" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F308" s="3">
         <v>66</v>
@@ -6230,7 +6356,7 @@
         <v>43</v>
       </c>
       <c r="D309" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F309" s="3">
         <v>66</v>
@@ -6244,7 +6370,7 @@
         <v>43</v>
       </c>
       <c r="D310" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F310" s="3">
         <v>66</v>
@@ -6258,7 +6384,7 @@
         <v>43</v>
       </c>
       <c r="D311" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F311" s="3">
         <v>66</v>
@@ -6272,7 +6398,7 @@
         <v>43</v>
       </c>
       <c r="D312" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F312" s="3">
         <v>66</v>
@@ -6286,7 +6412,7 @@
         <v>43</v>
       </c>
       <c r="D313" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F313" s="3">
         <v>67</v>
@@ -6294,7 +6420,7 @@
     </row>
     <row r="314" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B314" t="s">
         <v>3</v>
@@ -6308,17 +6434,113 @@
     </row>
     <row r="315" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="B315" t="s">
         <v>6</v>
       </c>
       <c r="D315" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F315" s="3">
         <v>71</v>
       </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A316" t="s">
+        <v>520</v>
+      </c>
+      <c r="B316" t="s">
+        <v>3</v>
+      </c>
+      <c r="C316" t="s">
+        <v>4</v>
+      </c>
+      <c r="D316" t="s">
+        <v>267</v>
+      </c>
+      <c r="F316" s="3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A317" t="s">
+        <v>522</v>
+      </c>
+      <c r="B317" t="s">
+        <v>515</v>
+      </c>
+      <c r="D317" t="s">
+        <v>267</v>
+      </c>
+      <c r="F317" s="3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A318" t="s">
+        <v>535</v>
+      </c>
+      <c r="B318" t="s">
+        <v>515</v>
+      </c>
+      <c r="D318" t="s">
+        <v>267</v>
+      </c>
+      <c r="F318" s="3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A319" t="s">
+        <v>537</v>
+      </c>
+      <c r="B319" t="s">
+        <v>515</v>
+      </c>
+      <c r="C319" t="s">
+        <v>4</v>
+      </c>
+      <c r="D319" t="s">
+        <v>267</v>
+      </c>
+      <c r="F319" s="3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A320" t="s">
+        <v>539</v>
+      </c>
+      <c r="B320" t="s">
+        <v>16</v>
+      </c>
+      <c r="D320" t="s">
+        <v>540</v>
+      </c>
+      <c r="F320" s="3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A321" t="s">
+        <v>542</v>
+      </c>
+      <c r="B321" t="s">
+        <v>3</v>
+      </c>
+      <c r="C321" t="s">
+        <v>4</v>
+      </c>
+      <c r="D321" t="s">
+        <v>543</v>
+      </c>
+      <c r="F321" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F322" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6327,10 +6549,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6544894E-BE1B-6143-B221-82724E45982C}">
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B87"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B77" sqref="B77"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6892,7 +7114,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
@@ -6900,7 +7122,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
@@ -6908,7 +7130,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
@@ -6916,7 +7138,119 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>517</v>
+        <v>514</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>545</v>
       </c>
     </row>
   </sheetData>

</xml_diff>